<commit_message>
Added more to MasterCollection.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/MasterCollection/MasterCollection.xlsx
+++ b/WorshipCreator.TestData/Source/Books/MasterCollection/MasterCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\MasterCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C73D8-7571-45A8-AFE3-BA6D951B47FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABF4CE5-0FF6-4951-8B74-F1957AE053F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CD347702-B65D-448E-9FF6-E909C95B2269}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$463</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$483</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4271" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4455" uniqueCount="945">
   <si>
     <t>Album #</t>
   </si>
@@ -2963,7 +2963,840 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="138">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3407,11 +4240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EFE7ADA-0055-40DD-889B-734737ABDB6A}">
-  <dimension ref="A1:X483"/>
+  <dimension ref="A1:Y483"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17667,7 +18499,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -17706,7 +18538,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
@@ -17722,8 +18554,29 @@
       <c r="E242" t="s">
         <v>512</v>
       </c>
+      <c r="G242" t="s">
+        <v>400</v>
+      </c>
+      <c r="H242" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I242" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J242" s="4">
+        <v>60</v>
+      </c>
+      <c r="K242" s="5" t="s">
+        <v>401</v>
+      </c>
       <c r="L242" s="10">
         <v>3350395</v>
+      </c>
+      <c r="M242" s="4">
+        <v>2001</v>
+      </c>
+      <c r="N242" s="4" t="s">
+        <v>402</v>
       </c>
       <c r="R242" t="s">
         <v>43</v>
@@ -17742,10 +18595,10 @@
 &amp;IF(H242=I242,""," "&amp;H242)
 &amp;IF(OR(Q242=I242,Q242=H242),""," "&amp;Q242)
 &amp;IF(Q242=R242,""," "&amp;R242)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">D </v>
+      </c>
+    </row>
+    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -17784,7 +18637,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -17823,7 +18676,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -17862,7 +18715,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -17901,7 +18754,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -17940,7 +18793,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -17979,7 +18832,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -18039,7 +18892,7 @@
         <v xml:space="preserve">A </v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -18078,7 +18931,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -18117,7 +18970,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -18156,7 +19009,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -18216,7 +19069,7 @@
         <v xml:space="preserve">D </v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -18232,8 +19085,29 @@
       <c r="E254" t="s">
         <v>524</v>
       </c>
-      <c r="L254" s="10">
-        <v>7036005</v>
+      <c r="G254" t="s">
+        <v>915</v>
+      </c>
+      <c r="H254" t="s">
+        <v>196</v>
+      </c>
+      <c r="I254" t="s">
+        <v>196</v>
+      </c>
+      <c r="J254">
+        <v>100</v>
+      </c>
+      <c r="K254" t="s">
+        <v>392</v>
+      </c>
+      <c r="L254" s="4">
+        <v>27721</v>
+      </c>
+      <c r="M254" s="10">
+        <v>1862</v>
+      </c>
+      <c r="N254" t="s">
+        <v>422</v>
       </c>
       <c r="R254" t="s">
         <v>43</v>
@@ -18252,10 +19126,13 @@
 &amp;IF(H254=I254,""," "&amp;H254)
 &amp;IF(OR(Q254=I254,Q254=H254),""," "&amp;Q254)
 &amp;IF(Q254=R254,""," "&amp;R254)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">F </v>
+      </c>
+      <c r="Y254" s="10">
+        <v>7036005</v>
+      </c>
+    </row>
+    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -18271,8 +19148,29 @@
       <c r="E255" t="s">
         <v>525</v>
       </c>
-      <c r="L255" s="10" t="s">
-        <v>944</v>
+      <c r="G255" t="s">
+        <v>925</v>
+      </c>
+      <c r="H255" t="s">
+        <v>45</v>
+      </c>
+      <c r="I255" t="s">
+        <v>45</v>
+      </c>
+      <c r="J255">
+        <v>110</v>
+      </c>
+      <c r="K255" t="s">
+        <v>392</v>
+      </c>
+      <c r="L255" s="4">
+        <v>31054</v>
+      </c>
+      <c r="M255" s="10">
+        <v>1841</v>
+      </c>
+      <c r="N255" t="s">
+        <v>422</v>
       </c>
       <c r="R255" t="s">
         <v>43</v>
@@ -18291,10 +19189,13 @@
 &amp;IF(H255=I255,""," "&amp;H255)
 &amp;IF(OR(Q255=I255,Q255=H255),""," "&amp;Q255)
 &amp;IF(Q255=R255,""," "&amp;R255)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">G </v>
+      </c>
+      <c r="Y255" s="10" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -18309,6 +19210,27 @@
       </c>
       <c r="E256" t="s">
         <v>526</v>
+      </c>
+      <c r="G256" t="s">
+        <v>917</v>
+      </c>
+      <c r="H256" t="s">
+        <v>196</v>
+      </c>
+      <c r="I256" t="s">
+        <v>196</v>
+      </c>
+      <c r="K256" t="s">
+        <v>392</v>
+      </c>
+      <c r="L256" s="4">
+        <v>29080</v>
+      </c>
+      <c r="M256" s="10">
+        <v>1909</v>
+      </c>
+      <c r="N256" t="s">
+        <v>422</v>
       </c>
       <c r="R256" t="s">
         <v>43</v>
@@ -18327,10 +19249,11 @@
 &amp;IF(H256=I256,""," "&amp;H256)
 &amp;IF(OR(Q256=I256,Q256=H256),""," "&amp;Q256)
 &amp;IF(Q256=R256,""," "&amp;R256)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">F </v>
+      </c>
+      <c r="Y256" s="10"/>
+    </row>
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
@@ -18345,6 +19268,30 @@
       </c>
       <c r="E257" t="s">
         <v>562</v>
+      </c>
+      <c r="G257" t="s">
+        <v>927</v>
+      </c>
+      <c r="H257" t="s">
+        <v>67</v>
+      </c>
+      <c r="I257" t="s">
+        <v>67</v>
+      </c>
+      <c r="J257">
+        <v>90</v>
+      </c>
+      <c r="K257" t="s">
+        <v>446</v>
+      </c>
+      <c r="L257" s="4">
+        <v>32015</v>
+      </c>
+      <c r="M257" s="10">
+        <v>1847</v>
+      </c>
+      <c r="N257" t="s">
+        <v>422</v>
       </c>
       <c r="R257" t="s">
         <v>43</v>
@@ -18363,10 +19310,11 @@
 &amp;IF(H257=I257,""," "&amp;H257)
 &amp;IF(OR(Q257=I257,Q257=H257),""," "&amp;Q257)
 &amp;IF(Q257=R257,""," "&amp;R257)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">C </v>
+      </c>
+      <c r="Y257" s="10"/>
+    </row>
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
@@ -18382,8 +19330,29 @@
       <c r="E258" t="s">
         <v>527</v>
       </c>
-      <c r="L258" s="10">
-        <v>7036006</v>
+      <c r="G258" t="s">
+        <v>880</v>
+      </c>
+      <c r="H258" t="s">
+        <v>59</v>
+      </c>
+      <c r="I258" t="s">
+        <v>59</v>
+      </c>
+      <c r="J258">
+        <v>96</v>
+      </c>
+      <c r="K258" t="s">
+        <v>921</v>
+      </c>
+      <c r="L258" s="4">
+        <v>24016</v>
+      </c>
+      <c r="M258" s="10">
+        <v>1719</v>
+      </c>
+      <c r="N258" t="s">
+        <v>422</v>
       </c>
       <c r="R258" t="s">
         <v>43</v>
@@ -18402,10 +19371,13 @@
 &amp;IF(H258=I258,""," "&amp;H258)
 &amp;IF(OR(Q258=I258,Q258=H258),""," "&amp;Q258)
 &amp;IF(Q258=R258,""," "&amp;R258)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">D </v>
+      </c>
+      <c r="Y258" s="10">
+        <v>7036006</v>
+      </c>
+    </row>
+    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
@@ -18421,8 +19393,26 @@
       <c r="E259" t="s">
         <v>528</v>
       </c>
-      <c r="L259" s="10">
-        <v>7036000</v>
+      <c r="G259" t="s">
+        <v>929</v>
+      </c>
+      <c r="H259" t="s">
+        <v>72</v>
+      </c>
+      <c r="I259" t="s">
+        <v>48</v>
+      </c>
+      <c r="K259" t="s">
+        <v>446</v>
+      </c>
+      <c r="L259" s="4">
+        <v>27862</v>
+      </c>
+      <c r="M259" s="10">
+        <v>1818</v>
+      </c>
+      <c r="N259" t="s">
+        <v>422</v>
       </c>
       <c r="R259" t="s">
         <v>43</v>
@@ -18441,10 +19431,13 @@
 &amp;IF(H259=I259,""," "&amp;H259)
 &amp;IF(OR(Q259=I259,Q259=H259),""," "&amp;Q259)
 &amp;IF(Q259=R259,""," "&amp;R259)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Bb A </v>
+      </c>
+      <c r="Y259" s="10">
+        <v>7036000</v>
+      </c>
+    </row>
+    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
@@ -18459,6 +19452,30 @@
       </c>
       <c r="E260" t="s">
         <v>563</v>
+      </c>
+      <c r="G260" t="s">
+        <v>918</v>
+      </c>
+      <c r="H260" t="s">
+        <v>59</v>
+      </c>
+      <c r="I260" t="s">
+        <v>59</v>
+      </c>
+      <c r="J260">
+        <v>80</v>
+      </c>
+      <c r="K260" t="s">
+        <v>401</v>
+      </c>
+      <c r="L260" s="4">
+        <v>31047</v>
+      </c>
+      <c r="M260" s="10">
+        <v>1833</v>
+      </c>
+      <c r="N260" t="s">
+        <v>422</v>
       </c>
       <c r="R260" t="s">
         <v>43</v>
@@ -18477,10 +19494,11 @@
 &amp;IF(H260=I260,""," "&amp;H260)
 &amp;IF(OR(Q260=I260,Q260=H260),""," "&amp;Q260)
 &amp;IF(Q260=R260,""," "&amp;R260)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">D </v>
+      </c>
+      <c r="Y260" s="10"/>
+    </row>
+    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
@@ -18495,6 +19513,30 @@
       </c>
       <c r="E261" t="s">
         <v>564</v>
+      </c>
+      <c r="G261" t="s">
+        <v>926</v>
+      </c>
+      <c r="H261" t="s">
+        <v>828</v>
+      </c>
+      <c r="I261" t="s">
+        <v>828</v>
+      </c>
+      <c r="J261">
+        <v>76</v>
+      </c>
+      <c r="K261" t="s">
+        <v>392</v>
+      </c>
+      <c r="L261" s="4">
+        <v>31982</v>
+      </c>
+      <c r="M261" s="10">
+        <v>1861</v>
+      </c>
+      <c r="N261" t="s">
+        <v>422</v>
       </c>
       <c r="R261" t="s">
         <v>43</v>
@@ -18513,10 +19555,11 @@
 &amp;IF(H261=I261,""," "&amp;H261)
 &amp;IF(OR(Q261=I261,Q261=H261),""," "&amp;Q261)
 &amp;IF(Q261=R261,""," "&amp;R261)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Em </v>
+      </c>
+      <c r="Y261" s="10"/>
+    </row>
+    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
@@ -18551,8 +19594,9 @@
 &amp;IF(Q262=R262,""," "&amp;R262)</f>
         <v/>
       </c>
-    </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y262" s="10"/>
+    </row>
+    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
@@ -18567,9 +19611,6 @@
       </c>
       <c r="E263" t="s">
         <v>529</v>
-      </c>
-      <c r="L263" s="10">
-        <v>7009580</v>
       </c>
       <c r="R263" t="s">
         <v>43</v>
@@ -18590,8 +19631,11 @@
 &amp;IF(Q263=R263,""," "&amp;R263)</f>
         <v/>
       </c>
-    </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y263" s="10">
+        <v>7009580</v>
+      </c>
+    </row>
+    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>263</v>
       </c>
@@ -18651,7 +19695,7 @@
         <v xml:space="preserve">F </v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
@@ -18690,7 +19734,7 @@
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
@@ -18706,8 +19750,26 @@
       <c r="E266" t="s">
         <v>532</v>
       </c>
-      <c r="L266" s="10">
-        <v>7104229</v>
+      <c r="G266" t="s">
+        <v>699</v>
+      </c>
+      <c r="H266" t="s">
+        <v>196</v>
+      </c>
+      <c r="I266" t="s">
+        <v>196</v>
+      </c>
+      <c r="K266" t="s">
+        <v>392</v>
+      </c>
+      <c r="L266" s="4">
+        <v>27738</v>
+      </c>
+      <c r="M266" s="10">
+        <v>1739</v>
+      </c>
+      <c r="N266" t="s">
+        <v>422</v>
       </c>
       <c r="R266" t="s">
         <v>43</v>
@@ -18726,10 +19788,13 @@
 &amp;IF(H266=I266,""," "&amp;H266)
 &amp;IF(OR(Q266=I266,Q266=H266),""," "&amp;Q266)
 &amp;IF(Q266=R266,""," "&amp;R266)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">F </v>
+      </c>
+      <c r="Y266" s="10">
+        <v>7104229</v>
+      </c>
+    </row>
+    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
@@ -18745,8 +19810,29 @@
       <c r="E267" t="s">
         <v>533</v>
       </c>
-      <c r="L267" s="10">
-        <v>7104272</v>
+      <c r="G267" t="s">
+        <v>928</v>
+      </c>
+      <c r="H267" t="s">
+        <v>196</v>
+      </c>
+      <c r="I267" t="s">
+        <v>196</v>
+      </c>
+      <c r="J267">
+        <v>90</v>
+      </c>
+      <c r="K267" t="s">
+        <v>392</v>
+      </c>
+      <c r="L267" s="4">
+        <v>27879</v>
+      </c>
+      <c r="M267" s="10">
+        <v>1868</v>
+      </c>
+      <c r="N267" t="s">
+        <v>422</v>
       </c>
       <c r="R267" t="s">
         <v>43</v>
@@ -18765,10 +19851,13 @@
 &amp;IF(H267=I267,""," "&amp;H267)
 &amp;IF(OR(Q267=I267,Q267=H267),""," "&amp;Q267)
 &amp;IF(Q267=R267,""," "&amp;R267)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">F </v>
+      </c>
+      <c r="Y267" s="10">
+        <v>7104272</v>
+      </c>
+    </row>
+    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
@@ -18783,9 +19872,6 @@
       </c>
       <c r="E268" t="s">
         <v>534</v>
-      </c>
-      <c r="L268" s="10">
-        <v>1128784</v>
       </c>
       <c r="R268" t="s">
         <v>43</v>
@@ -18806,8 +19892,11 @@
 &amp;IF(Q268=R268,""," "&amp;R268)</f>
         <v/>
       </c>
-    </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y268" s="10">
+        <v>1128784</v>
+      </c>
+    </row>
+    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
@@ -18822,9 +19911,6 @@
       </c>
       <c r="E269" t="s">
         <v>535</v>
-      </c>
-      <c r="L269" s="10">
-        <v>7121311</v>
       </c>
       <c r="R269" t="s">
         <v>43</v>
@@ -18845,8 +19931,11 @@
 &amp;IF(Q269=R269,""," "&amp;R269)</f>
         <v/>
       </c>
-    </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y269" s="10">
+        <v>7121311</v>
+      </c>
+    </row>
+    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
@@ -18862,8 +19951,26 @@
       <c r="E270" t="s">
         <v>536</v>
       </c>
-      <c r="L270" s="10">
-        <v>7104268</v>
+      <c r="G270" t="s">
+        <v>931</v>
+      </c>
+      <c r="H270" t="s">
+        <v>45</v>
+      </c>
+      <c r="I270" t="s">
+        <v>45</v>
+      </c>
+      <c r="K270" t="s">
+        <v>446</v>
+      </c>
+      <c r="L270" s="4">
+        <v>30983</v>
+      </c>
+      <c r="M270" s="10">
+        <v>1865</v>
+      </c>
+      <c r="N270" t="s">
+        <v>422</v>
       </c>
       <c r="R270" t="s">
         <v>43</v>
@@ -18882,10 +19989,13 @@
 &amp;IF(H270=I270,""," "&amp;H270)
 &amp;IF(OR(Q270=I270,Q270=H270),""," "&amp;Q270)
 &amp;IF(Q270=R270,""," "&amp;R270)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">G </v>
+      </c>
+      <c r="Y270" s="10">
+        <v>7104268</v>
+      </c>
+    </row>
+    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
@@ -18945,7 +20055,7 @@
         <v xml:space="preserve">F </v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
@@ -18960,9 +20070,6 @@
       </c>
       <c r="E272" t="s">
         <v>538</v>
-      </c>
-      <c r="L272" s="10">
-        <v>5492031</v>
       </c>
       <c r="R272" t="s">
         <v>43</v>
@@ -18983,8 +20090,11 @@
 &amp;IF(Q272=R272,""," "&amp;R272)</f>
         <v/>
       </c>
-    </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y272" s="10">
+        <v>5492031</v>
+      </c>
+    </row>
+    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
@@ -19000,8 +20110,29 @@
       <c r="E273" t="s">
         <v>539</v>
       </c>
-      <c r="L273" s="10">
-        <v>7104270</v>
+      <c r="G273" t="s">
+        <v>920</v>
+      </c>
+      <c r="H273" t="s">
+        <v>45</v>
+      </c>
+      <c r="I273" t="s">
+        <v>87</v>
+      </c>
+      <c r="J273">
+        <v>120</v>
+      </c>
+      <c r="K273" t="s">
+        <v>446</v>
+      </c>
+      <c r="L273" s="4">
+        <v>31078</v>
+      </c>
+      <c r="M273" s="10">
+        <v>1849</v>
+      </c>
+      <c r="N273" t="s">
+        <v>422</v>
       </c>
       <c r="R273" t="s">
         <v>43</v>
@@ -19020,10 +20151,13 @@
 &amp;IF(H273=I273,""," "&amp;H273)
 &amp;IF(OR(Q273=I273,Q273=H273),""," "&amp;Q273)
 &amp;IF(Q273=R273,""," "&amp;R273)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Ab G </v>
+      </c>
+      <c r="Y273" s="10">
+        <v>7104270</v>
+      </c>
+    </row>
+    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
@@ -19062,7 +20196,7 @@
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
@@ -19101,7 +20235,7 @@
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
@@ -19140,7 +20274,7 @@
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
@@ -19179,7 +20313,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -19218,7 +20352,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -19257,7 +20391,7 @@
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
@@ -19296,7 +20430,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
@@ -19335,7 +20469,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
@@ -19374,7 +20508,7 @@
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
@@ -19413,7 +20547,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
@@ -19452,7 +20586,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
@@ -19491,7 +20625,7 @@
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
@@ -19530,7 +20664,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
@@ -19569,7 +20703,7 @@
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
@@ -22233,6 +23367,9 @@
     <row r="365" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>364</v>
+      </c>
+      <c r="D365" t="s">
+        <v>896</v>
       </c>
       <c r="E365" t="s">
         <v>685</v>
@@ -22286,6 +23423,9 @@
       <c r="A366">
         <v>365</v>
       </c>
+      <c r="D366" t="s">
+        <v>896</v>
+      </c>
       <c r="E366" t="s">
         <v>686</v>
       </c>
@@ -22338,6 +23478,9 @@
       <c r="A367">
         <v>366</v>
       </c>
+      <c r="D367" t="s">
+        <v>896</v>
+      </c>
       <c r="E367" t="s">
         <v>687</v>
       </c>
@@ -22390,6 +23533,9 @@
       <c r="A368">
         <v>367</v>
       </c>
+      <c r="D368" t="s">
+        <v>896</v>
+      </c>
       <c r="E368" t="s">
         <v>688</v>
       </c>
@@ -22442,6 +23588,9 @@
       <c r="A369">
         <v>368</v>
       </c>
+      <c r="D369" t="s">
+        <v>896</v>
+      </c>
       <c r="E369" t="s">
         <v>694</v>
       </c>
@@ -22494,6 +23643,9 @@
       <c r="A370">
         <v>369</v>
       </c>
+      <c r="D370" t="s">
+        <v>896</v>
+      </c>
       <c r="E370" t="s">
         <v>164</v>
       </c>
@@ -22546,6 +23698,9 @@
       <c r="A371">
         <v>370</v>
       </c>
+      <c r="D371" t="s">
+        <v>896</v>
+      </c>
       <c r="E371" t="s">
         <v>696</v>
       </c>
@@ -22598,6 +23753,9 @@
       <c r="A372">
         <v>371</v>
       </c>
+      <c r="D372" t="s">
+        <v>896</v>
+      </c>
       <c r="E372" t="s">
         <v>697</v>
       </c>
@@ -22653,6 +23811,9 @@
       <c r="A373">
         <v>372</v>
       </c>
+      <c r="D373" t="s">
+        <v>896</v>
+      </c>
       <c r="E373" t="s">
         <v>700</v>
       </c>
@@ -22705,6 +23866,9 @@
       <c r="A374">
         <v>373</v>
       </c>
+      <c r="D374" t="s">
+        <v>896</v>
+      </c>
       <c r="E374" t="s">
         <v>701</v>
       </c>
@@ -22757,6 +23921,9 @@
       <c r="A375">
         <v>374</v>
       </c>
+      <c r="D375" t="s">
+        <v>896</v>
+      </c>
       <c r="E375" t="s">
         <v>222</v>
       </c>
@@ -22809,6 +23976,9 @@
       <c r="A376">
         <v>375</v>
       </c>
+      <c r="D376" t="s">
+        <v>896</v>
+      </c>
       <c r="E376" t="s">
         <v>706</v>
       </c>
@@ -22859,6 +24029,9 @@
       <c r="A377">
         <v>376</v>
       </c>
+      <c r="D377" t="s">
+        <v>896</v>
+      </c>
       <c r="E377" t="s">
         <v>708</v>
       </c>
@@ -22911,6 +24084,9 @@
       <c r="A378">
         <v>377</v>
       </c>
+      <c r="D378" t="s">
+        <v>896</v>
+      </c>
       <c r="E378" t="s">
         <v>709</v>
       </c>
@@ -22963,6 +24139,9 @@
       <c r="A379">
         <v>378</v>
       </c>
+      <c r="D379" t="s">
+        <v>896</v>
+      </c>
       <c r="E379" t="s">
         <v>329</v>
       </c>
@@ -23015,6 +24194,9 @@
       <c r="A380">
         <v>379</v>
       </c>
+      <c r="D380" t="s">
+        <v>896</v>
+      </c>
       <c r="E380" t="s">
         <v>715</v>
       </c>
@@ -23067,6 +24249,9 @@
       <c r="A381">
         <v>380</v>
       </c>
+      <c r="D381" t="s">
+        <v>896</v>
+      </c>
       <c r="E381" t="s">
         <v>718</v>
       </c>
@@ -23119,6 +24304,9 @@
       <c r="A382">
         <v>381</v>
       </c>
+      <c r="D382" t="s">
+        <v>896</v>
+      </c>
       <c r="E382" t="s">
         <v>719</v>
       </c>
@@ -23171,6 +24359,9 @@
       <c r="A383">
         <v>382</v>
       </c>
+      <c r="D383" t="s">
+        <v>896</v>
+      </c>
       <c r="E383" t="s">
         <v>722</v>
       </c>
@@ -23223,6 +24414,9 @@
       <c r="A384">
         <v>383</v>
       </c>
+      <c r="D384" t="s">
+        <v>896</v>
+      </c>
       <c r="E384" t="s">
         <v>722</v>
       </c>
@@ -23279,6 +24473,9 @@
     <row r="385" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>384</v>
+      </c>
+      <c r="D385" t="s">
+        <v>896</v>
       </c>
       <c r="E385" t="s">
         <v>724</v>
@@ -23332,6 +24529,9 @@
       <c r="A386">
         <v>385</v>
       </c>
+      <c r="D386" t="s">
+        <v>896</v>
+      </c>
       <c r="E386" t="s">
         <v>60</v>
       </c>
@@ -23384,6 +24584,9 @@
       <c r="A387">
         <v>386</v>
       </c>
+      <c r="D387" t="s">
+        <v>896</v>
+      </c>
       <c r="E387" t="s">
         <v>728</v>
       </c>
@@ -23439,6 +24642,9 @@
       <c r="A388">
         <v>387</v>
       </c>
+      <c r="D388" t="s">
+        <v>896</v>
+      </c>
       <c r="E388" t="s">
         <v>523</v>
       </c>
@@ -23491,6 +24697,9 @@
       <c r="A389">
         <v>388</v>
       </c>
+      <c r="D389" t="s">
+        <v>896</v>
+      </c>
       <c r="E389" t="s">
         <v>729</v>
       </c>
@@ -23543,6 +24752,9 @@
       <c r="A390">
         <v>389</v>
       </c>
+      <c r="D390" t="s">
+        <v>896</v>
+      </c>
       <c r="E390" t="s">
         <v>734</v>
       </c>
@@ -23595,6 +24807,9 @@
       <c r="A391">
         <v>390</v>
       </c>
+      <c r="D391" t="s">
+        <v>896</v>
+      </c>
       <c r="E391" t="s">
         <v>327</v>
       </c>
@@ -23647,6 +24862,9 @@
       <c r="A392">
         <v>391</v>
       </c>
+      <c r="D392" t="s">
+        <v>896</v>
+      </c>
       <c r="E392" t="s">
         <v>738</v>
       </c>
@@ -23699,6 +24917,9 @@
       <c r="A393">
         <v>392</v>
       </c>
+      <c r="D393" t="s">
+        <v>896</v>
+      </c>
       <c r="E393" t="s">
         <v>740</v>
       </c>
@@ -23751,6 +24972,9 @@
       <c r="A394">
         <v>393</v>
       </c>
+      <c r="D394" t="s">
+        <v>896</v>
+      </c>
       <c r="E394" t="s">
         <v>742</v>
       </c>
@@ -23804,6 +25028,9 @@
     <row r="395" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>394</v>
+      </c>
+      <c r="D395" t="s">
+        <v>896</v>
       </c>
       <c r="E395" t="s">
         <v>134</v>
@@ -23860,6 +25087,9 @@
       <c r="A396">
         <v>395</v>
       </c>
+      <c r="D396" t="s">
+        <v>896</v>
+      </c>
       <c r="E396" t="s">
         <v>316</v>
       </c>
@@ -23916,6 +25146,9 @@
     <row r="397" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>396</v>
+      </c>
+      <c r="D397" t="s">
+        <v>896</v>
       </c>
       <c r="E397" t="s">
         <v>747</v>
@@ -23969,6 +25202,9 @@
       <c r="A398">
         <v>397</v>
       </c>
+      <c r="D398" t="s">
+        <v>896</v>
+      </c>
       <c r="E398" t="s">
         <v>752</v>
       </c>
@@ -24021,6 +25257,9 @@
       <c r="A399">
         <v>398</v>
       </c>
+      <c r="D399" t="s">
+        <v>896</v>
+      </c>
       <c r="E399" t="s">
         <v>754</v>
       </c>
@@ -24073,6 +25312,9 @@
       <c r="A400">
         <v>399</v>
       </c>
+      <c r="D400" t="s">
+        <v>896</v>
+      </c>
       <c r="E400" t="s">
         <v>755</v>
       </c>
@@ -24129,6 +25371,9 @@
     <row r="401" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>400</v>
+      </c>
+      <c r="D401" t="s">
+        <v>896</v>
       </c>
       <c r="E401" t="s">
         <v>757</v>
@@ -24180,6 +25425,9 @@
       <c r="A402">
         <v>401</v>
       </c>
+      <c r="D402" t="s">
+        <v>896</v>
+      </c>
       <c r="E402" t="s">
         <v>73</v>
       </c>
@@ -24232,6 +25480,9 @@
       <c r="A403">
         <v>402</v>
       </c>
+      <c r="D403" t="s">
+        <v>896</v>
+      </c>
       <c r="E403" t="s">
         <v>763</v>
       </c>
@@ -24284,6 +25535,9 @@
       <c r="A404">
         <v>403</v>
       </c>
+      <c r="D404" t="s">
+        <v>896</v>
+      </c>
       <c r="E404" t="s">
         <v>505</v>
       </c>
@@ -24336,6 +25590,9 @@
       <c r="A405">
         <v>404</v>
       </c>
+      <c r="D405" t="s">
+        <v>896</v>
+      </c>
       <c r="E405" t="s">
         <v>765</v>
       </c>
@@ -24388,6 +25645,9 @@
       <c r="A406">
         <v>405</v>
       </c>
+      <c r="D406" t="s">
+        <v>896</v>
+      </c>
       <c r="E406" t="s">
         <v>766</v>
       </c>
@@ -24440,6 +25700,9 @@
       <c r="A407">
         <v>406</v>
       </c>
+      <c r="D407" t="s">
+        <v>896</v>
+      </c>
       <c r="E407" t="s">
         <v>767</v>
       </c>
@@ -24492,6 +25755,9 @@
       <c r="A408">
         <v>407</v>
       </c>
+      <c r="D408" t="s">
+        <v>896</v>
+      </c>
       <c r="E408" t="s">
         <v>101</v>
       </c>
@@ -24547,6 +25813,9 @@
       <c r="A409">
         <v>408</v>
       </c>
+      <c r="D409" t="s">
+        <v>896</v>
+      </c>
       <c r="E409" t="s">
         <v>769</v>
       </c>
@@ -24599,6 +25868,9 @@
       <c r="A410">
         <v>409</v>
       </c>
+      <c r="D410" t="s">
+        <v>896</v>
+      </c>
       <c r="E410" t="s">
         <v>778</v>
       </c>
@@ -24651,6 +25923,9 @@
       <c r="A411">
         <v>410</v>
       </c>
+      <c r="D411" t="s">
+        <v>896</v>
+      </c>
       <c r="E411" t="s">
         <v>779</v>
       </c>
@@ -24703,6 +25978,9 @@
       <c r="A412">
         <v>411</v>
       </c>
+      <c r="D412" t="s">
+        <v>896</v>
+      </c>
       <c r="E412" t="s">
         <v>780</v>
       </c>
@@ -24755,6 +26033,9 @@
       <c r="A413">
         <v>412</v>
       </c>
+      <c r="D413" t="s">
+        <v>896</v>
+      </c>
       <c r="E413" t="s">
         <v>785</v>
       </c>
@@ -24805,6 +26086,9 @@
       <c r="A414">
         <v>413</v>
       </c>
+      <c r="D414" t="s">
+        <v>896</v>
+      </c>
       <c r="E414" t="s">
         <v>786</v>
       </c>
@@ -24855,6 +26139,9 @@
       <c r="A415">
         <v>414</v>
       </c>
+      <c r="D415" t="s">
+        <v>896</v>
+      </c>
       <c r="E415" t="s">
         <v>787</v>
       </c>
@@ -24908,6 +26195,9 @@
     <row r="416" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>415</v>
+      </c>
+      <c r="D416" t="s">
+        <v>896</v>
       </c>
       <c r="E416" t="s">
         <v>791</v>
@@ -24961,6 +26251,9 @@
       <c r="A417">
         <v>416</v>
       </c>
+      <c r="D417" t="s">
+        <v>896</v>
+      </c>
       <c r="E417" t="s">
         <v>792</v>
       </c>
@@ -25013,6 +26306,9 @@
       <c r="A418">
         <v>417</v>
       </c>
+      <c r="D418" t="s">
+        <v>896</v>
+      </c>
       <c r="E418" t="s">
         <v>792</v>
       </c>
@@ -25068,6 +26364,9 @@
       <c r="A419">
         <v>418</v>
       </c>
+      <c r="D419" t="s">
+        <v>896</v>
+      </c>
       <c r="E419" t="s">
         <v>798</v>
       </c>
@@ -25123,6 +26422,9 @@
       <c r="A420">
         <v>419</v>
       </c>
+      <c r="D420" t="s">
+        <v>896</v>
+      </c>
       <c r="E420" t="s">
         <v>800</v>
       </c>
@@ -25175,6 +26477,9 @@
       <c r="A421">
         <v>420</v>
       </c>
+      <c r="D421" t="s">
+        <v>896</v>
+      </c>
       <c r="E421" t="s">
         <v>801</v>
       </c>
@@ -25227,6 +26532,9 @@
       <c r="A422">
         <v>421</v>
       </c>
+      <c r="D422" t="s">
+        <v>896</v>
+      </c>
       <c r="E422" t="s">
         <v>804</v>
       </c>
@@ -25277,6 +26585,9 @@
       <c r="A423">
         <v>422</v>
       </c>
+      <c r="D423" t="s">
+        <v>896</v>
+      </c>
       <c r="E423" t="s">
         <v>806</v>
       </c>
@@ -25329,6 +26640,9 @@
       <c r="A424">
         <v>423</v>
       </c>
+      <c r="D424" t="s">
+        <v>896</v>
+      </c>
       <c r="E424" t="s">
         <v>808</v>
       </c>
@@ -25381,6 +26695,9 @@
       <c r="A425">
         <v>424</v>
       </c>
+      <c r="D425" t="s">
+        <v>896</v>
+      </c>
       <c r="E425" t="s">
         <v>810</v>
       </c>
@@ -25433,6 +26750,9 @@
       <c r="A426">
         <v>425</v>
       </c>
+      <c r="D426" t="s">
+        <v>896</v>
+      </c>
       <c r="E426" t="s">
         <v>186</v>
       </c>
@@ -25483,6 +26803,9 @@
       <c r="A427">
         <v>426</v>
       </c>
+      <c r="D427" t="s">
+        <v>896</v>
+      </c>
       <c r="E427" t="s">
         <v>814</v>
       </c>
@@ -25538,6 +26861,9 @@
       <c r="A428">
         <v>427</v>
       </c>
+      <c r="D428" t="s">
+        <v>896</v>
+      </c>
       <c r="E428" t="s">
         <v>816</v>
       </c>
@@ -25590,6 +26916,9 @@
       <c r="A429">
         <v>428</v>
       </c>
+      <c r="D429" t="s">
+        <v>896</v>
+      </c>
       <c r="E429" t="s">
         <v>816</v>
       </c>
@@ -25645,6 +26974,9 @@
       <c r="A430">
         <v>429</v>
       </c>
+      <c r="D430" t="s">
+        <v>896</v>
+      </c>
       <c r="E430" t="s">
         <v>818</v>
       </c>
@@ -25697,6 +27029,9 @@
       <c r="A431">
         <v>430</v>
       </c>
+      <c r="D431" t="s">
+        <v>896</v>
+      </c>
       <c r="E431" t="s">
         <v>819</v>
       </c>
@@ -25749,6 +27084,9 @@
       <c r="A432">
         <v>431</v>
       </c>
+      <c r="D432" t="s">
+        <v>896</v>
+      </c>
       <c r="E432" t="s">
         <v>820</v>
       </c>
@@ -25801,6 +27139,9 @@
       <c r="A433">
         <v>432</v>
       </c>
+      <c r="D433" t="s">
+        <v>896</v>
+      </c>
       <c r="E433" t="s">
         <v>825</v>
       </c>
@@ -25853,6 +27194,9 @@
       <c r="A434">
         <v>433</v>
       </c>
+      <c r="D434" t="s">
+        <v>896</v>
+      </c>
       <c r="E434" t="s">
         <v>826</v>
       </c>
@@ -25905,6 +27249,9 @@
       <c r="A435">
         <v>434</v>
       </c>
+      <c r="D435" t="s">
+        <v>896</v>
+      </c>
       <c r="E435" t="s">
         <v>829</v>
       </c>
@@ -25958,6 +27305,9 @@
     <row r="436" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>435</v>
+      </c>
+      <c r="D436" t="s">
+        <v>896</v>
       </c>
       <c r="E436" t="s">
         <v>830</v>
@@ -26011,6 +27361,9 @@
       <c r="A437">
         <v>436</v>
       </c>
+      <c r="D437" t="s">
+        <v>896</v>
+      </c>
       <c r="E437" t="s">
         <v>831</v>
       </c>
@@ -26063,6 +27416,9 @@
       <c r="A438">
         <v>437</v>
       </c>
+      <c r="D438" t="s">
+        <v>896</v>
+      </c>
       <c r="E438" t="s">
         <v>833</v>
       </c>
@@ -26115,6 +27471,9 @@
       <c r="A439">
         <v>438</v>
       </c>
+      <c r="D439" t="s">
+        <v>896</v>
+      </c>
       <c r="E439" t="s">
         <v>834</v>
       </c>
@@ -26167,6 +27526,9 @@
       <c r="A440">
         <v>439</v>
       </c>
+      <c r="D440" t="s">
+        <v>896</v>
+      </c>
       <c r="E440" t="s">
         <v>835</v>
       </c>
@@ -26220,6 +27582,9 @@
     <row r="441" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>440</v>
+      </c>
+      <c r="D441" t="s">
+        <v>896</v>
       </c>
       <c r="E441" t="s">
         <v>839</v>
@@ -26273,6 +27638,9 @@
       <c r="A442">
         <v>441</v>
       </c>
+      <c r="D442" t="s">
+        <v>896</v>
+      </c>
       <c r="E442" t="s">
         <v>842</v>
       </c>
@@ -26325,6 +27693,9 @@
       <c r="A443">
         <v>442</v>
       </c>
+      <c r="D443" t="s">
+        <v>896</v>
+      </c>
       <c r="E443" t="s">
         <v>845</v>
       </c>
@@ -26377,6 +27748,9 @@
       <c r="A444">
         <v>443</v>
       </c>
+      <c r="D444" t="s">
+        <v>896</v>
+      </c>
       <c r="E444" t="s">
         <v>847</v>
       </c>
@@ -26432,6 +27806,9 @@
       <c r="A445">
         <v>444</v>
       </c>
+      <c r="D445" t="s">
+        <v>896</v>
+      </c>
       <c r="E445" t="s">
         <v>849</v>
       </c>
@@ -26485,6 +27862,9 @@
     <row r="446" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>445</v>
+      </c>
+      <c r="D446" t="s">
+        <v>896</v>
       </c>
       <c r="E446" t="s">
         <v>850</v>
@@ -26538,6 +27918,9 @@
       <c r="A447">
         <v>446</v>
       </c>
+      <c r="D447" t="s">
+        <v>896</v>
+      </c>
       <c r="E447" t="s">
         <v>851</v>
       </c>
@@ -26590,6 +27973,9 @@
       <c r="A448">
         <v>447</v>
       </c>
+      <c r="D448" t="s">
+        <v>896</v>
+      </c>
       <c r="E448" t="s">
         <v>852</v>
       </c>
@@ -26642,6 +28028,9 @@
       <c r="A449">
         <v>448</v>
       </c>
+      <c r="D449" t="s">
+        <v>896</v>
+      </c>
       <c r="E449" t="s">
         <v>857</v>
       </c>
@@ -26694,6 +28083,9 @@
       <c r="A450">
         <v>449</v>
       </c>
+      <c r="D450" t="s">
+        <v>896</v>
+      </c>
       <c r="E450" t="s">
         <v>858</v>
       </c>
@@ -26746,6 +28138,9 @@
       <c r="A451">
         <v>450</v>
       </c>
+      <c r="D451" t="s">
+        <v>896</v>
+      </c>
       <c r="E451" t="s">
         <v>859</v>
       </c>
@@ -26798,6 +28193,9 @@
       <c r="A452">
         <v>451</v>
       </c>
+      <c r="D452" t="s">
+        <v>896</v>
+      </c>
       <c r="E452" t="s">
         <v>864</v>
       </c>
@@ -26850,6 +28248,9 @@
       <c r="A453">
         <v>452</v>
       </c>
+      <c r="D453" t="s">
+        <v>896</v>
+      </c>
       <c r="E453" t="s">
         <v>865</v>
       </c>
@@ -26902,6 +28303,9 @@
       <c r="A454">
         <v>453</v>
       </c>
+      <c r="D454" t="s">
+        <v>896</v>
+      </c>
       <c r="E454" t="s">
         <v>866</v>
       </c>
@@ -26957,6 +28361,9 @@
       <c r="A455">
         <v>454</v>
       </c>
+      <c r="D455" t="s">
+        <v>896</v>
+      </c>
       <c r="E455" t="s">
         <v>868</v>
       </c>
@@ -27009,6 +28416,9 @@
       <c r="A456">
         <v>455</v>
       </c>
+      <c r="D456" t="s">
+        <v>896</v>
+      </c>
       <c r="E456" t="s">
         <v>869</v>
       </c>
@@ -27061,6 +28471,9 @@
       <c r="A457">
         <v>456</v>
       </c>
+      <c r="D457" t="s">
+        <v>896</v>
+      </c>
       <c r="E457" t="s">
         <v>877</v>
       </c>
@@ -27113,6 +28526,9 @@
       <c r="A458">
         <v>457</v>
       </c>
+      <c r="D458" t="s">
+        <v>896</v>
+      </c>
       <c r="E458" t="s">
         <v>878</v>
       </c>
@@ -27165,6 +28581,9 @@
       <c r="A459">
         <v>458</v>
       </c>
+      <c r="D459" t="s">
+        <v>896</v>
+      </c>
       <c r="E459" t="s">
         <v>879</v>
       </c>
@@ -27218,6 +28637,9 @@
     <row r="460" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>459</v>
+      </c>
+      <c r="D460" t="s">
+        <v>896</v>
       </c>
       <c r="E460" t="s">
         <v>883</v>
@@ -27271,6 +28693,9 @@
       <c r="A461">
         <v>460</v>
       </c>
+      <c r="D461" t="s">
+        <v>896</v>
+      </c>
       <c r="E461" t="s">
         <v>886</v>
       </c>
@@ -27326,6 +28751,9 @@
       <c r="A462">
         <v>461</v>
       </c>
+      <c r="D462" t="s">
+        <v>896</v>
+      </c>
       <c r="E462" t="s">
         <v>888</v>
       </c>
@@ -27381,6 +28809,9 @@
       <c r="A463">
         <v>462</v>
       </c>
+      <c r="D463" t="s">
+        <v>896</v>
+      </c>
       <c r="E463" t="s">
         <v>894</v>
       </c>
@@ -27433,6 +28864,9 @@
       <c r="A464">
         <v>463</v>
       </c>
+      <c r="D464" t="s">
+        <v>943</v>
+      </c>
       <c r="E464" t="s">
         <v>933</v>
       </c>
@@ -27481,6 +28915,9 @@
       <c r="A465">
         <v>464</v>
       </c>
+      <c r="D465" t="s">
+        <v>943</v>
+      </c>
       <c r="E465" t="s">
         <v>524</v>
       </c>
@@ -27529,6 +28966,9 @@
       <c r="A466">
         <v>465</v>
       </c>
+      <c r="D466" t="s">
+        <v>943</v>
+      </c>
       <c r="E466" t="s">
         <v>934</v>
       </c>
@@ -27577,6 +29017,9 @@
       <c r="A467">
         <v>466</v>
       </c>
+      <c r="D467" t="s">
+        <v>943</v>
+      </c>
       <c r="E467" t="s">
         <v>530</v>
       </c>
@@ -27625,6 +29068,9 @@
       <c r="A468">
         <v>467</v>
       </c>
+      <c r="D468" t="s">
+        <v>943</v>
+      </c>
       <c r="E468" t="s">
         <v>526</v>
       </c>
@@ -27670,6 +29116,9 @@
       <c r="A469">
         <v>468</v>
       </c>
+      <c r="D469" t="s">
+        <v>943</v>
+      </c>
       <c r="E469" t="s">
         <v>935</v>
       </c>
@@ -27718,6 +29167,9 @@
       <c r="A470">
         <v>469</v>
       </c>
+      <c r="D470" t="s">
+        <v>943</v>
+      </c>
       <c r="E470" t="s">
         <v>936</v>
       </c>
@@ -27766,6 +29218,9 @@
       <c r="A471">
         <v>470</v>
       </c>
+      <c r="D471" t="s">
+        <v>943</v>
+      </c>
       <c r="E471" t="s">
         <v>937</v>
       </c>
@@ -27811,6 +29266,9 @@
       <c r="A472">
         <v>471</v>
       </c>
+      <c r="D472" t="s">
+        <v>943</v>
+      </c>
       <c r="E472" t="s">
         <v>938</v>
       </c>
@@ -27859,6 +29317,9 @@
       <c r="A473">
         <v>472</v>
       </c>
+      <c r="D473" t="s">
+        <v>943</v>
+      </c>
       <c r="E473" t="s">
         <v>527</v>
       </c>
@@ -27907,6 +29368,9 @@
       <c r="A474">
         <v>473</v>
       </c>
+      <c r="D474" t="s">
+        <v>943</v>
+      </c>
       <c r="E474" t="s">
         <v>939</v>
       </c>
@@ -27952,6 +29416,9 @@
       <c r="A475">
         <v>474</v>
       </c>
+      <c r="D475" t="s">
+        <v>943</v>
+      </c>
       <c r="E475" t="s">
         <v>525</v>
       </c>
@@ -28000,6 +29467,9 @@
       <c r="A476">
         <v>475</v>
       </c>
+      <c r="D476" t="s">
+        <v>943</v>
+      </c>
       <c r="E476" t="s">
         <v>564</v>
       </c>
@@ -28048,6 +29518,9 @@
       <c r="A477">
         <v>476</v>
       </c>
+      <c r="D477" t="s">
+        <v>943</v>
+      </c>
       <c r="E477" t="s">
         <v>562</v>
       </c>
@@ -28096,6 +29569,9 @@
       <c r="A478">
         <v>477</v>
       </c>
+      <c r="D478" t="s">
+        <v>943</v>
+      </c>
       <c r="E478" t="s">
         <v>940</v>
       </c>
@@ -28144,6 +29620,9 @@
       <c r="A479">
         <v>478</v>
       </c>
+      <c r="D479" t="s">
+        <v>943</v>
+      </c>
       <c r="E479" t="s">
         <v>528</v>
       </c>
@@ -28189,6 +29668,9 @@
       <c r="A480">
         <v>479</v>
       </c>
+      <c r="D480" t="s">
+        <v>943</v>
+      </c>
       <c r="E480" t="s">
         <v>563</v>
       </c>
@@ -28237,6 +29719,9 @@
       <c r="A481">
         <v>480</v>
       </c>
+      <c r="D481" t="s">
+        <v>943</v>
+      </c>
       <c r="E481" t="s">
         <v>941</v>
       </c>
@@ -28285,6 +29770,9 @@
       <c r="A482">
         <v>481</v>
       </c>
+      <c r="D482" t="s">
+        <v>943</v>
+      </c>
       <c r="E482" t="s">
         <v>536</v>
       </c>
@@ -28330,6 +29818,9 @@
       <c r="A483">
         <v>482</v>
       </c>
+      <c r="D483" t="s">
+        <v>943</v>
+      </c>
       <c r="E483" t="s">
         <v>942</v>
       </c>
@@ -28375,43 +29866,148 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X463" xr:uid="{5714BB12-8592-4F7C-AFEC-0DD1045CE9C9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X483">
-      <sortCondition ref="A1:A463"/>
+  <autoFilter ref="A1:Y483" xr:uid="{2120240A-6AEB-4B0B-9C4B-AFD525A5CB3B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y483">
+      <sortCondition ref="A1:A483"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X483">
     <sortCondition ref="L2:L483"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="48"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L365:L483">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="L2:L483">
+    <cfRule type="duplicateValues" dxfId="89" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L68">
+    <cfRule type="duplicateValues" dxfId="85" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L136">
+    <cfRule type="duplicateValues" dxfId="84" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L315">
+    <cfRule type="duplicateValues" dxfId="83" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L254">
+    <cfRule type="duplicateValues" dxfId="82" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L254">
+    <cfRule type="duplicateValues" dxfId="81" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L255">
+    <cfRule type="duplicateValues" dxfId="80" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L255">
+    <cfRule type="duplicateValues" dxfId="79" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L256">
+    <cfRule type="duplicateValues" dxfId="78" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L256">
+    <cfRule type="duplicateValues" dxfId="77" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L257">
+    <cfRule type="duplicateValues" dxfId="76" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L257">
+    <cfRule type="duplicateValues" dxfId="75" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L258">
+    <cfRule type="duplicateValues" dxfId="74" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L258">
+    <cfRule type="duplicateValues" dxfId="73" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L259">
+    <cfRule type="duplicateValues" dxfId="72" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L259">
+    <cfRule type="duplicateValues" dxfId="71" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L260">
+    <cfRule type="duplicateValues" dxfId="70" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L260">
+    <cfRule type="duplicateValues" dxfId="69" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L261">
+    <cfRule type="duplicateValues" dxfId="68" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L261">
+    <cfRule type="duplicateValues" dxfId="67" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L266">
+    <cfRule type="duplicateValues" dxfId="66" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L266">
+    <cfRule type="duplicateValues" dxfId="65" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L267">
+    <cfRule type="duplicateValues" dxfId="64" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L267">
+    <cfRule type="duplicateValues" dxfId="63" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L270">
+    <cfRule type="duplicateValues" dxfId="62" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L270">
+    <cfRule type="duplicateValues" dxfId="61" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L273">
+    <cfRule type="duplicateValues" dxfId="60" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L273">
+    <cfRule type="duplicateValues" dxfId="59" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L34">
+    <cfRule type="duplicateValues" dxfId="58" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L45">
+    <cfRule type="duplicateValues" dxfId="57" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L47">
+    <cfRule type="duplicateValues" dxfId="56" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L50">
+    <cfRule type="duplicateValues" dxfId="55" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52">
+    <cfRule type="duplicateValues" dxfId="54" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L56">
+    <cfRule type="duplicateValues" dxfId="53" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L60">
+    <cfRule type="duplicateValues" dxfId="52" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L68">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="L64">
+    <cfRule type="duplicateValues" dxfId="50" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L136">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="L66">
+    <cfRule type="duplicateValues" dxfId="49" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L315">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="L71">
+    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76">
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L126">
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated spreadsheets to indicate album art status, and have consistent names.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/MasterCollection/MasterCollection.xlsx
+++ b/WorshipCreator.TestData/Source/Books/MasterCollection/MasterCollection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\MasterCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B6FB6E-45A0-463A-B416-37C81D5D4002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DC0133-A9D1-4342-895A-3064F1375C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{CD347702-B65D-448E-9FF6-E909C95B2269}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CD347702-B65D-448E-9FF6-E909C95B2269}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="3" r:id="rId1"/>
@@ -3084,7 +3084,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3124,6 +3124,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8411,7 +8417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000E114C-5757-48D5-BC32-E094B4022FC3}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9130,7 +9136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EFE7ADA-0055-40DD-889B-734737ABDB6A}">
   <dimension ref="A1:AB465"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -40013,6 +40019,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA465">
     <sortCondition ref="L2:L465"/>
   </sortState>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="E279:E1048576 E1:E277">
     <cfRule type="duplicateValues" dxfId="44" priority="48"/>
   </conditionalFormatting>

</xml_diff>